<commit_message>
Open chain 2nd stage version commit
</commit_message>
<xml_diff>
--- a/Open chain project/chaindata.xlsx
+++ b/Open chain project/chaindata.xlsx
@@ -644,14 +644,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">

</xml_diff>